<commit_message>
Update Vaccine alert BDD scenarios.xlsx
</commit_message>
<xml_diff>
--- a/Vaccine alert BDD scenarios.xlsx
+++ b/Vaccine alert BDD scenarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggurung\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\GitHub\codecraft_exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8020D7F-5F21-4753-A1C2-C409EE3B763B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FC643B-A35B-4189-9B1D-BC8B87E7FDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="3210" windowWidth="27780" windowHeight="15225" activeTab="2" xr2:uid="{394E7A85-FE8A-4D92-93B5-8EFE2E07C975}"/>
   </bookViews>
@@ -18,6 +18,8 @@
     <sheet name="scenario 1" sheetId="3" r:id="rId3"/>
     <sheet name="scenario 2" sheetId="4" r:id="rId4"/>
     <sheet name="scenario 3" sheetId="5" r:id="rId5"/>
+    <sheet name="scenario 4" sheetId="6" r:id="rId6"/>
+    <sheet name="scenario 5" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="46">
   <si>
     <t>GIVEN</t>
   </si>
@@ -163,6 +165,21 @@
   </si>
   <si>
     <t>don't push any notification to customer</t>
+  </si>
+  <si>
+    <t>Scenario: Don't send a reminder if last administered vaccine is not avaiable</t>
+  </si>
+  <si>
+    <t>the date of the last administered vaccine is NOT available</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>vaccine interval is NOT defined</t>
+  </si>
+  <si>
+    <t>Scenario: Don't send a reminder if vaccine interval is not avaiable</t>
   </si>
 </sst>
 </file>
@@ -218,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,9 +245,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -248,17 +262,23 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,32 +626,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -689,32 +709,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -729,17 +749,17 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -780,88 +800,88 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>46055</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -870,12 +890,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -886,7 +906,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,32 +918,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -938,24 +958,24 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1005,94 +1025,94 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>45658</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
         <v>45996</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>46023</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1112,7 +1132,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,32 +1144,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1164,24 +1184,24 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1231,94 +1251,540 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>45809</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
         <v>45996</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>46174</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31370593-5C43-4724-A0B9-8181DDE4C969}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45658</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
+        <v>45996</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>46023</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F2F1A1-5621-456F-9593-CA7BBA1B1FB5}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
+        <v>45996</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>46023</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1338,12 +1804,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31370593-5C43-4724-A0B9-8181DDE4C969}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B2C3FA-1B9E-4D17-A67E-0F6A59FA4BDA}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,64 +1821,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="1"/>
+      <c r="A4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1421,7 +1887,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1454,94 +1920,94 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>45658</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>30</v>
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
         <v>45996</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="A25" s="11">
         <v>46023</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>

</xml_diff>